<commit_message>
poprawa formuł na wycenie. Bez zmiany danych.
</commit_message>
<xml_diff>
--- a/Wycena.xlsx
+++ b/Wycena.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Właściciel\Desktop\Unity.git\trunk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Unity Projects\SVN-Unity\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2138,7 +2138,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,15 +2240,15 @@
         <v>4</v>
       </c>
       <c r="I2" s="9">
-        <f t="shared" ref="I2:I41" si="0">IF(ISNUMBER($H2),$H2/8,"")</f>
-        <v>0.5</v>
+        <f>IF(ISNUMBER($H2),$H2/4,"")</f>
+        <v>1</v>
       </c>
       <c r="J2" s="8">
-        <f t="shared" ref="J2:J33" si="1">IF(AND(ISNUMBER($H2), $B2=100%),$H2-$F2,"")</f>
+        <f t="shared" ref="J2:J33" si="0">IF(AND(ISNUMBER($H2), $B2=100%),$H2-$F2,"")</f>
         <v>0</v>
       </c>
       <c r="K2" s="9">
-        <f t="shared" ref="K2:K33" si="2">IF(ISNUMBER($J2),$J2/8,"")</f>
+        <f t="shared" ref="K2:K33" si="1">IF(ISNUMBER($J2),$J2/8,"")</f>
         <v>0</v>
       </c>
       <c r="L2" s="4"/>
@@ -2293,22 +2293,22 @@
         <v>3</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G52" si="3">IF(ISNUMBER($F3),$F3/4,"")</f>
+        <f t="shared" ref="G3:G52" si="2">IF(ISNUMBER($F3),$F3/4,"")</f>
         <v>0.75</v>
       </c>
       <c r="H3" s="21">
         <v>1</v>
       </c>
       <c r="I3" s="9">
+        <f t="shared" ref="I3:I52" si="3">IF(ISNUMBER($H3),$H3/4,"")</f>
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-      <c r="J3" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K3" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K3" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L3" s="4"/>
@@ -2344,22 +2344,22 @@
         <v>2</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="H4" s="21">
         <v>1</v>
       </c>
       <c r="I4" s="9">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-      <c r="J4" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K4" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K4" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L4" s="4"/>
@@ -2385,22 +2385,22 @@
         <v>10</v>
       </c>
       <c r="G5" s="7">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
         <f t="shared" si="3"/>
-        <v>2.5</v>
-      </c>
-      <c r="H5" s="21">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K5" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K5" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L5" s="4"/>
@@ -2426,22 +2426,22 @@
         <v>10</v>
       </c>
       <c r="G6" s="7">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
         <f t="shared" si="3"/>
-        <v>2.5</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K6" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K6" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L6" s="4"/>
@@ -2467,18 +2467,18 @@
         <v>10</v>
       </c>
       <c r="G7" s="7">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
         <f t="shared" si="3"/>
-        <v>2.5</v>
-      </c>
-      <c r="H7" s="21">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K7" s="9" t="str">
@@ -2508,18 +2508,18 @@
         <v>1</v>
       </c>
       <c r="G8" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="H8" s="21">
         <v>2</v>
       </c>
       <c r="I8" s="9">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="8">
         <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="J8" s="8">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K8" s="9">
@@ -2547,18 +2547,18 @@
         <v>2</v>
       </c>
       <c r="G9" s="7">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="21">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K9" s="9" t="str">
@@ -2588,18 +2588,18 @@
         <v>8</v>
       </c>
       <c r="G10" s="7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="H10" s="21">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K10" s="9" t="str">
@@ -2627,18 +2627,18 @@
         <v>12</v>
       </c>
       <c r="G11" s="7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="H11" s="21">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K11" s="9" t="str">
@@ -2668,22 +2668,22 @@
         <v>3</v>
       </c>
       <c r="G12" s="7">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="H12" s="21">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
         <f t="shared" si="3"/>
-        <v>0.75</v>
-      </c>
-      <c r="H12" s="21">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K12" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K12" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L12" s="4"/>
@@ -2709,18 +2709,18 @@
         <v>4</v>
       </c>
       <c r="G13" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H13" s="21">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K13" s="9"/>
@@ -2745,16 +2745,16 @@
         <v>4</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J14" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J14" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K14" s="9"/>
@@ -2781,20 +2781,20 @@
         <v>60</v>
       </c>
       <c r="G15" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J15" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J15" s="8" t="str">
+      <c r="K15" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K15" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L15" s="4"/>
@@ -2825,20 +2825,20 @@
         <v>30</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="H16" s="21"/>
       <c r="I16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J16" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J16" s="8" t="str">
+      <c r="K16" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K16" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L16" s="4"/>
@@ -2867,18 +2867,18 @@
         <v>6</v>
       </c>
       <c r="G17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="H17" s="21">
         <v>8</v>
       </c>
       <c r="I17" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J17" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J17" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K17" s="9"/>
@@ -2905,16 +2905,16 @@
         <v>20</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J18" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J18" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K18" s="9"/>
@@ -2941,16 +2941,16 @@
         <v>30</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="H19" s="21"/>
       <c r="I19" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J19" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J19" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K19" s="9"/>
@@ -2977,16 +2977,16 @@
         <v>10</v>
       </c>
       <c r="G20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="H20" s="21"/>
       <c r="I20" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J20" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J20" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K20" s="9"/>
@@ -3011,16 +3011,16 @@
         <v>4</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H21" s="21"/>
       <c r="I21" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J21" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J21" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K21" s="9"/>
@@ -3045,20 +3045,20 @@
         <v>4</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J22" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J22" s="8" t="str">
+      <c r="K22" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K22" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L22" s="4"/>
@@ -3082,20 +3082,20 @@
         <v>2</v>
       </c>
       <c r="G23" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="H23" s="21"/>
       <c r="I23" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J23" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J23" s="8" t="str">
+      <c r="K23" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K23" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L23" s="4"/>
@@ -3121,20 +3121,20 @@
         <v>4</v>
       </c>
       <c r="G24" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J24" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J24" s="8" t="str">
+      <c r="K24" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K24" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L24" s="4"/>
@@ -3160,16 +3160,16 @@
         <v>4</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J25" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J25" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K25" s="9" t="str">
@@ -3199,16 +3199,16 @@
         <v>8</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H26" s="21"/>
       <c r="I26" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J26" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J26" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K26" s="9" t="str">
@@ -3230,16 +3230,16 @@
       <c r="E27" s="12"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J27" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J27" s="8" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K27" s="9" t="str">
@@ -3261,20 +3261,20 @@
       <c r="E28" s="19"/>
       <c r="F28" s="20"/>
       <c r="G28" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J28" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J28" s="8" t="str">
+      <c r="K28" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K28" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L28" s="4"/>
@@ -3292,20 +3292,20 @@
       <c r="E29" s="19"/>
       <c r="F29" s="20"/>
       <c r="G29" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H29" s="21"/>
       <c r="I29" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J29" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J29" s="8" t="str">
+      <c r="K29" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K29" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L29" s="4"/>
@@ -3323,20 +3323,20 @@
       <c r="E30" s="19"/>
       <c r="F30" s="20"/>
       <c r="G30" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H30" s="21"/>
       <c r="I30" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J30" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J30" s="8" t="str">
+      <c r="K30" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K30" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L30" s="4"/>
@@ -3354,20 +3354,20 @@
       <c r="E31" s="19"/>
       <c r="F31" s="20"/>
       <c r="G31" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H31" s="21"/>
       <c r="I31" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J31" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J31" s="8" t="str">
+      <c r="K31" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K31" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L31" s="4"/>
@@ -3383,22 +3383,22 @@
       <c r="C32" s="29"/>
       <c r="D32" s="11"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H32" s="14"/>
       <c r="I32" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J32" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J32" s="8" t="str">
+      <c r="K32" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K32" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L32" s="4"/>
@@ -3416,20 +3416,20 @@
       <c r="E33" s="12"/>
       <c r="F33" s="20"/>
       <c r="G33" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H33" s="21"/>
       <c r="I33" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J33" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J33" s="8" t="str">
+      <c r="K33" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K33" s="9" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L33" s="4"/>
@@ -3447,12 +3447,12 @@
       <c r="E34" s="12"/>
       <c r="F34" s="20"/>
       <c r="G34" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H34" s="21"/>
       <c r="I34" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J34" s="8" t="str">
@@ -3478,12 +3478,12 @@
       <c r="E35" s="12"/>
       <c r="F35" s="20"/>
       <c r="G35" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H35" s="21"/>
       <c r="I35" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J35" s="8" t="str">
@@ -3509,12 +3509,12 @@
       <c r="E36" s="12"/>
       <c r="F36" s="20"/>
       <c r="G36" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H36" s="21"/>
       <c r="I36" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J36" s="8" t="str">
@@ -3538,17 +3538,14 @@
       <c r="C37" s="29"/>
       <c r="D37" s="18"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="20">
-        <f>SUM(F2:F26)</f>
-        <v>255</v>
-      </c>
-      <c r="G37" s="7">
-        <f t="shared" si="3"/>
-        <v>63.75</v>
+      <c r="F37" s="20"/>
+      <c r="G37" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J37" s="8" t="str">
@@ -3574,12 +3571,12 @@
       <c r="E38" s="12"/>
       <c r="F38" s="20"/>
       <c r="G38" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H38" s="21"/>
       <c r="I38" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J38" s="8" t="str">
@@ -3605,12 +3602,12 @@
       <c r="E39" s="12"/>
       <c r="F39" s="20"/>
       <c r="G39" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J39" s="8" t="str">
@@ -3636,12 +3633,12 @@
       <c r="E40" s="12"/>
       <c r="F40" s="20"/>
       <c r="G40" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H40" s="21"/>
       <c r="I40" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J40" s="8" t="str">
@@ -3667,12 +3664,12 @@
       <c r="E41" s="12"/>
       <c r="F41" s="20"/>
       <c r="G41" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H41" s="21"/>
       <c r="I41" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J41" s="8" t="str">
@@ -3698,12 +3695,12 @@
       <c r="E42" s="12"/>
       <c r="F42" s="20"/>
       <c r="G42" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H42" s="21"/>
       <c r="I42" s="9" t="str">
-        <f t="shared" ref="I42:I52" si="8">IF(ISNUMBER($H42),$H42/8,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J42" s="8" t="str">
@@ -3729,12 +3726,12 @@
       <c r="E43" s="12"/>
       <c r="F43" s="20"/>
       <c r="G43" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H43" s="21"/>
       <c r="I43" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J43" s="8" t="str">
@@ -3760,12 +3757,12 @@
       <c r="E44" s="12"/>
       <c r="F44" s="20"/>
       <c r="G44" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H44" s="21"/>
       <c r="I44" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J44" s="8" t="str">
@@ -3791,12 +3788,12 @@
       <c r="E45" s="12"/>
       <c r="F45" s="20"/>
       <c r="G45" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H45" s="21"/>
       <c r="I45" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J45" s="8" t="str">
@@ -3819,12 +3816,12 @@
       <c r="E46" s="12"/>
       <c r="F46" s="20"/>
       <c r="G46" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H46" s="21"/>
       <c r="I46" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J46" s="8" t="str">
@@ -3847,12 +3844,12 @@
       <c r="E47" s="12"/>
       <c r="F47" s="20"/>
       <c r="G47" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H47" s="21"/>
       <c r="I47" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J47" s="8" t="str">
@@ -3875,12 +3872,12 @@
       <c r="E48" s="12"/>
       <c r="F48" s="20"/>
       <c r="G48" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H48" s="21"/>
       <c r="I48" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J48" s="8" t="str">
@@ -3903,12 +3900,12 @@
       <c r="E49" s="12"/>
       <c r="F49" s="20"/>
       <c r="G49" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H49" s="21"/>
       <c r="I49" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J49" s="8" t="str">
@@ -3931,12 +3928,12 @@
       <c r="E50" s="12"/>
       <c r="F50" s="20"/>
       <c r="G50" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H50" s="21"/>
       <c r="I50" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J50" s="8" t="str">
@@ -3944,7 +3941,7 @@
         <v/>
       </c>
       <c r="K50" s="9" t="str">
-        <f t="shared" ref="K50:K52" si="9">IF(ISNUMBER($J50),$J50/8,"")</f>
+        <f t="shared" ref="K50:K52" si="8">IF(ISNUMBER($J50),$J50/8,"")</f>
         <v/>
       </c>
       <c r="L50" s="4"/>
@@ -3962,12 +3959,12 @@
       <c r="E51" s="12"/>
       <c r="F51" s="20"/>
       <c r="G51" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H51" s="21"/>
       <c r="I51" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J51" s="8" t="str">
@@ -3975,7 +3972,7 @@
         <v/>
       </c>
       <c r="K51" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L51" s="4"/>
@@ -3991,12 +3988,12 @@
       <c r="E52" s="25"/>
       <c r="F52" s="26"/>
       <c r="G52" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H52" s="27"/>
+      <c r="I52" s="9" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H52" s="27"/>
-      <c r="I52" s="28" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J52" s="27" t="str">
@@ -4004,7 +4001,7 @@
         <v/>
       </c>
       <c r="K52" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L52" s="4"/>
@@ -4026,11 +4023,11 @@
       <c r="E53" s="15"/>
       <c r="F53" s="15">
         <f>SUM(F2:F52)</f>
-        <v>510</v>
+        <v>255</v>
       </c>
       <c r="G53" s="15">
         <f>SUM(G2:G52)</f>
-        <v>127.5</v>
+        <v>63.75</v>
       </c>
       <c r="H53" s="15">
         <f>SUM(H2:H51)</f>
@@ -4038,7 +4035,7 @@
       </c>
       <c r="I53" s="15">
         <f>SUM(I2:I51)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J53" s="15">
         <f>SUM(J2:J51)</f>

</xml_diff>